<commit_message>
Added Framework to GetTableCellTextTest
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
   <si>
     <t xml:space="preserve">Company</t>
   </si>
@@ -46,6 +46,21 @@
     <t xml:space="preserve">Magazzini Alimentari Riuniti</t>
   </si>
   <si>
+    <t xml:space="preserve">Eliran Duveen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdfdh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h5f23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdgvr dsrgr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/.,/rty5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Contact</t>
   </si>
   <si>
@@ -67,6 +82,18 @@
     <t xml:space="preserve">Giovanni Rovelli</t>
   </si>
   <si>
+    <t xml:space="preserve">sgdsgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'lih[oi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cs;kljdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f234thh6;</t>
+  </si>
+  <si>
     <t xml:space="preserve">Country</t>
   </si>
   <si>
@@ -86,6 +113,15 @@
   </si>
   <si>
     <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Israel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gdeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nhfjh345</t>
   </si>
 </sst>
 </file>
@@ -448,10 +484,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="1" sqref="A13 A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -516,19 +552,45 @@
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -546,10 +608,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="A13 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -560,37 +622,72 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -609,10 +706,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -623,37 +720,67 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -675,7 +802,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A13 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -690,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,10 +828,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,10 +839,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,10 +850,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,10 +861,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,10 +872,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,10 +883,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added framework to VerifyTableCellTextTest
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Company" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t xml:space="preserve">Company</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">nhfjh345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
   </si>
 </sst>
 </file>
@@ -622,8 +619,8 @@
   </sheetPr>
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="1" sqref="A15 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -725,7 +722,7 @@
   </sheetPr>
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -802,12 +799,12 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -829,7 +826,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="A15 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>